<commit_message>
Rectified the ShareSkil and Manage Listing
</commit_message>
<xml_diff>
--- a/SpecflowPM.Tests/ExcelTestData/ShareSkillData.xlsx
+++ b/SpecflowPM.Tests/ExcelTestData/ShareSkillData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinky Sindhu\Desktop\Industry Connect\Industry Connect\Internship\Task 2\marsframework-master\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinky Sindhu\Desktop\Industry Connect\Industry Connect\Internship\Task 3\ProjectMars.QA\SpecflowPM.Tests\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE9FFA-6108-4B94-8128-3B7386397C7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9654C654-37E8-45FD-95B2-62F4E38B3192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{47384E78-1A99-4AD6-B104-C46CFD79473E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Email</t>
   </si>
@@ -140,10 +140,16 @@
     <t>8:00:00 PM</t>
   </si>
   <si>
-    <t>14/04/2021</t>
-  </si>
-  <si>
-    <t>20/05/2021</t>
+    <t>14/06/2021</t>
+  </si>
+  <si>
+    <t>20/08/2021</t>
+  </si>
+  <si>
+    <t>Cypress</t>
+  </si>
+  <si>
+    <t>Would like to provide Cypress training for beginners</t>
   </si>
 </sst>
 </file>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854EB62A-56E0-4A62-AC5F-55A15B29C1B5}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -686,6 +692,106 @@
         <v>19</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>